<commit_message>
added proportion of total
</commit_message>
<xml_diff>
--- a/2023_summary_data.xlsx
+++ b/2023_summary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.VanHorn\Work\GitHub\AnnRpt-FMA-OLE-Chapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B363F133-9785-48A9-8A60-D31B48823E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{449C5CBA-1B07-43B7-B770-92F5AC3794DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="By New Statement Type" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="104">
   <si>
     <t>CONTRACTOR REQUIREMENTS</t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>Catcher Processor Longline</t>
+  </si>
+  <si>
+    <t>Proportion of Total</t>
   </si>
 </sst>
 </file>
@@ -739,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -927,6 +930,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -972,7 +1012,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1034,34 +1074,88 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1443,7 +1537,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1464,7 +1558,7 @@
       <c r="C1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2110,145 +2204,198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="25" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="25" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" style="23" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C1" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="30">
         <f>SUM('By New Statement Type'!C2:C3)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C2" s="43">
+        <f>B2/B14</f>
+        <v>2.5943396226415096E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="31">
         <f>SUM('By New Statement Type'!C4:C7)</f>
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C3" s="44">
+        <f>B3/B14</f>
+        <v>0.12028301886792453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="32">
         <f>SUM('By New Statement Type'!C8:C12)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="10">
+        <f>B4/B14</f>
+        <v>5.1886792452830191E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="33">
         <f>SUM('By New Statement Type'!C13:C14)</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C5" s="11">
+        <f>B5/B14</f>
+        <v>6.8396226415094338E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="34">
         <f>SUM('By New Statement Type'!C15:C22)</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C6" s="12">
+        <f>B6/B14</f>
+        <v>0.15330188679245282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="35">
         <f>SUM('By New Statement Type'!C23:C30)</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="C7" s="13">
+        <f>B7/B14</f>
+        <v>6.6037735849056603E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="36">
         <f>SUM('By New Statement Type'!C31:C34)</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="C8" s="14">
+        <f>B8/B14</f>
+        <v>0.10849056603773585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="37">
         <f>SUM('By New Statement Type'!C35:C40)</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C9" s="15">
+        <f>B9/B14</f>
+        <v>0.14858490566037735</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="38">
         <f>SUM('By New Statement Type'!C41:C43)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="C10" s="16">
+        <f>B10/B14</f>
+        <v>3.5377358490566037E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="39">
         <f>SUM('By New Statement Type'!C44)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C11" s="17">
+        <f>B11/B14</f>
+        <v>3.3018867924528301E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="40">
         <f>SUM('By New Statement Type'!C45)</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C12" s="18">
+        <f>B12/B14</f>
+        <v>0.14386792452830188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="41">
         <f>SUM('By New Statement Type'!C46)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="25" t="s">
+      <c r="C13" s="19">
+        <f>B13/B14</f>
+        <v>4.4811320754716978E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="23">
         <f>SUM(B2:B13)</f>
         <v>424</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2256,7 +2403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2269,16 +2416,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="28" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2507,13 +2654,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="25">
         <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -2521,13 +2668,13 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="25">
         <v>7</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2535,13 +2682,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="25">
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -2549,13 +2696,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="25">
         <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -2591,13 +2738,13 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="26">
         <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -2605,13 +2752,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="26">
         <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2619,13 +2766,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="26">
         <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -2633,13 +2780,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="26">
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -2647,13 +2794,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="26">
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -2661,13 +2808,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="26">
         <v>25</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -2675,13 +2822,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="26">
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -2689,13 +2836,13 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="26">
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -2703,13 +2850,13 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="26">
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -2728,81 +2875,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.08984375" style="6" customWidth="1"/>
     <col min="2" max="2" width="17.08984375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="45" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="C1" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="46">
         <f>SUM('By Old Statement Type (2023)'!C2:C9)</f>
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="27">
+        <f>B2/B8</f>
+        <v>0.29753914988814317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="36">
         <f>SUM('By Old Statement Type (2023)'!C10:C13)</f>
         <v>126</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C3" s="14">
+        <f>B3/B8</f>
+        <v>0.28187919463087246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="37">
         <f>SUM('By Old Statement Type (2023)'!C14:C17)</f>
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="27" t="s">
+      <c r="C4" s="15">
+        <f>B4/B8</f>
+        <v>0.12304250559284116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="47">
         <f>SUM('By Old Statement Type (2023)'!C18:C21)</f>
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C5" s="25">
+        <f>B5/B8</f>
+        <v>8.2774049217002238E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="34">
         <f>SUM('By Old Statement Type (2023)'!C22:C23)</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="28" t="s">
+      <c r="C6" s="12">
+        <f>B6/B8</f>
+        <v>6.7114093959731544E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="48">
         <f>SUM('By Old Statement Type (2023)'!C24:C32)</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="26">
+        <f>B7/B8</f>
+        <v>0.1476510067114094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
updated for corrected data
statements_combined updated to remove duplicated data points (by summing), removed 2024 (unaffected here)
</commit_message>
<xml_diff>
--- a/2023_summary_data.xlsx
+++ b/2023_summary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.VanHorn\Work\GitHub\AnnRpt-FMA-OLE-Chapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{449C5CBA-1B07-43B7-B770-92F5AC3794DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{36E94CCD-74D2-4133-A9DB-FAD7D6BECEA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="By New Statement Type" sheetId="1" r:id="rId1"/>
@@ -1536,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1584,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>100</v>
@@ -1612,7 +1612,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="9">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>100</v>
@@ -1626,7 +1626,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="9">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>100</v>
@@ -2032,7 +2032,7 @@
         <v>41</v>
       </c>
       <c r="C35" s="15">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>100</v>
@@ -2088,7 +2088,7 @@
         <v>45</v>
       </c>
       <c r="C39" s="15">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>100</v>
@@ -2186,7 +2186,7 @@
         <v>56</v>
       </c>
       <c r="C46" s="19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>100</v>
@@ -2207,7 +2207,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2234,11 +2234,11 @@
       </c>
       <c r="B2" s="30">
         <f>SUM('By New Statement Type'!C2:C3)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="43">
         <f>B2/B14</f>
-        <v>2.5943396226415096E-2</v>
+        <v>2.2113022113022112E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2247,11 +2247,11 @@
       </c>
       <c r="B3" s="31">
         <f>SUM('By New Statement Type'!C4:C7)</f>
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C3" s="44">
         <f>B3/B14</f>
-        <v>0.12028301886792453</v>
+        <v>0.10319410319410319</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="C4" s="10">
         <f>B4/B14</f>
-        <v>5.1886792452830191E-2</v>
+        <v>5.4054054054054057E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="C5" s="11">
         <f>B5/B14</f>
-        <v>6.8396226415094338E-2</v>
+        <v>7.125307125307126E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="C6" s="12">
         <f>B6/B14</f>
-        <v>0.15330188679245282</v>
+        <v>0.15970515970515969</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="C7" s="13">
         <f>B7/B14</f>
-        <v>6.6037735849056603E-2</v>
+        <v>6.8796068796068796E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="C8" s="14">
         <f>B8/B14</f>
-        <v>0.10849056603773585</v>
+        <v>0.11302211302211303</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
@@ -2325,11 +2325,11 @@
       </c>
       <c r="B9" s="37">
         <f>SUM('By New Statement Type'!C35:C40)</f>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C9" s="15">
         <f>B9/B14</f>
-        <v>0.14858490566037735</v>
+        <v>0.14250614250614252</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="C10" s="16">
         <f>B10/B14</f>
-        <v>3.5377358490566037E-2</v>
+        <v>3.6855036855036855E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" x14ac:dyDescent="0.35">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="C11" s="17">
         <f>B11/B14</f>
-        <v>3.3018867924528301E-2</v>
+        <v>3.4398034398034398E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="C12" s="18">
         <f>B12/B14</f>
-        <v>0.14386792452830188</v>
+        <v>0.14987714987714987</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2377,11 +2377,11 @@
       </c>
       <c r="B13" s="41">
         <f>SUM('By New Statement Type'!C46)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="19">
         <f>B13/B14</f>
-        <v>4.4811320754716978E-2</v>
+        <v>4.4226044226044224E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="B14" s="23">
         <f>SUM(B2:B13)</f>
-        <v>424</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2877,7 +2877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>